<commit_message>
style/doc: Commented code and filled in info about the single-cell data in DesignMatrix.xlsx
</commit_message>
<xml_diff>
--- a/data/DesignMatrix.xlsx
+++ b/data/DesignMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE25D358-ABB6-6B45-B493-48D179C45444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F1CF4-768B-46B5-816C-D1F7E34E6699}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="241">
   <si>
     <t>Sample index</t>
   </si>
@@ -631,6 +631,129 @@
   </si>
   <si>
     <t>Mix T cell</t>
+  </si>
+  <si>
+    <t>HCA CB</t>
+  </si>
+  <si>
+    <t>CB1T</t>
+  </si>
+  <si>
+    <t>CB2T</t>
+  </si>
+  <si>
+    <t>CB3T</t>
+  </si>
+  <si>
+    <t>CB4T</t>
+  </si>
+  <si>
+    <t>CB5T</t>
+  </si>
+  <si>
+    <t>CB6T</t>
+  </si>
+  <si>
+    <t>CB7T</t>
+  </si>
+  <si>
+    <t>CB8T</t>
+  </si>
+  <si>
+    <t>CB1B</t>
+  </si>
+  <si>
+    <t>CB2B</t>
+  </si>
+  <si>
+    <t>CB3B</t>
+  </si>
+  <si>
+    <t>CB4B</t>
+  </si>
+  <si>
+    <t>CB5B</t>
+  </si>
+  <si>
+    <t>CB6B</t>
+  </si>
+  <si>
+    <t>CB7B</t>
+  </si>
+  <si>
+    <t>CB8B</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>LCPat3T</t>
+  </si>
+  <si>
+    <t>LCPat4T</t>
+  </si>
+  <si>
+    <t>LCPat5T</t>
+  </si>
+  <si>
+    <t>LCPat3B</t>
+  </si>
+  <si>
+    <t>LCPat4B</t>
+  </si>
+  <si>
+    <t>LCPat5B</t>
+  </si>
+  <si>
+    <t>LCHT</t>
+  </si>
+  <si>
+    <t>LCHB</t>
+  </si>
+  <si>
+    <t>From tumor</t>
+  </si>
+  <si>
+    <t>From healthy tissue</t>
+  </si>
+  <si>
+    <t>PBMC68k</t>
+  </si>
+  <si>
+    <t>PBMC68kT</t>
+  </si>
+  <si>
+    <t>PBMC68kB</t>
+  </si>
+  <si>
+    <t>TCD4MEM</t>
+  </si>
+  <si>
+    <t>B10k</t>
+  </si>
+  <si>
+    <t>TCD8</t>
+  </si>
+  <si>
+    <t>T-Cells, CD4+ memory</t>
+  </si>
+  <si>
+    <t>T-Cells, CD8+</t>
+  </si>
+  <si>
+    <t>FACS-sorted</t>
+  </si>
+  <si>
+    <t>MELT</t>
+  </si>
+  <si>
+    <t>MELB</t>
+  </si>
+  <si>
+    <t>MEL</t>
+  </si>
+  <si>
+    <t>Smart-Seq2</t>
   </si>
 </sst>
 </file>
@@ -991,18 +1114,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
   <dimension ref="B2:DC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="CO4" sqref="CO4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="107" width="3.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="107" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:107" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1145,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1342,7 +1465,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1662,7 +1785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1982,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
@@ -2302,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -2462,7 +2585,7 @@
       <c r="DB7" s="4"/>
       <c r="DC7" s="4"/>
     </row>
-    <row r="8" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2782,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>188</v>
       </c>
@@ -3102,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:107" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>56</v>
       </c>
@@ -3241,9 +3364,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3251,7 +3374,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3266,23 +3389,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3302,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3322,7 +3445,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3342,7 +3465,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3362,7 +3485,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3382,7 +3505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3402,7 +3525,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3422,7 +3545,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3442,7 +3565,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3462,7 +3585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3482,7 +3605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3502,7 +3625,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3522,7 +3645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3542,7 +3665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3560,7 +3683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3576,7 +3699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3592,7 +3715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3610,7 +3733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3626,7 +3749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3642,7 +3765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3660,7 +3783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3676,7 +3799,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3692,7 +3815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3710,7 +3833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3726,7 +3849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3742,7 +3865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3762,7 +3885,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3782,7 +3905,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3802,7 +3925,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3822,7 +3945,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3842,7 +3965,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3862,7 +3985,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3882,7 +4005,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3902,7 +4025,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3922,7 +4045,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3942,7 +4065,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3962,7 +4085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3982,7 +4105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4002,7 +4125,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4022,7 +4145,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4042,7 +4165,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4062,7 +4185,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4082,7 +4205,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4102,7 +4225,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4122,7 +4245,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4142,7 +4265,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4162,7 +4285,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4182,7 +4305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4202,7 +4325,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4222,7 +4345,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4242,7 +4365,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4262,7 +4385,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -4282,7 +4405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4302,7 +4425,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4322,7 +4445,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4342,7 +4465,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4362,7 +4485,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4382,7 +4505,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4402,7 +4525,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4422,7 +4545,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4442,7 +4565,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4462,7 +4585,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4482,7 +4605,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4502,7 +4625,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4522,7 +4645,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4542,7 +4665,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4559,7 +4682,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4573,7 +4696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4587,7 +4710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4601,7 +4724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4615,7 +4738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4629,7 +4752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4643,7 +4766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4657,7 +4780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4671,7 +4794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4683,6 +4806,479 @@
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C76" t="s">
+        <v>201</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C78" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C80" t="s">
+        <v>205</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C81" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C82" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C83" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C85" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" t="s">
+        <v>211</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" t="s">
+        <v>212</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C88" t="s">
+        <v>213</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" t="s">
+        <v>214</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" t="s">
+        <v>215</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C94" t="s">
+        <v>220</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C95" t="s">
+        <v>221</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" t="s">
+        <v>222</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" t="s">
+        <v>223</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C98" t="s">
+        <v>224</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C99" t="s">
+        <v>225</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C100" t="s">
+        <v>229</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C101" t="s">
+        <v>230</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -4699,9 +5295,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4709,7 +5305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4717,7 +5313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4725,7 +5321,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4746,9 +5342,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4756,7 +5352,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4764,7 +5360,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4772,7 +5368,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4780,7 +5376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4791,7 +5387,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4799,7 +5395,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4807,7 +5403,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4815,7 +5411,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4823,7 +5419,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4840,13 +5436,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6499CB2B-6832-4092-A9EA-DD66A17F48BA}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4854,7 +5450,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4862,7 +5458,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4870,7 +5466,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4878,7 +5474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4886,7 +5482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4894,7 +5490,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4902,7 +5498,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4910,7 +5506,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4918,7 +5514,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4926,7 +5522,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4934,7 +5530,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4942,7 +5538,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
feat: Changed to variancePartition and added deconvolution analysis. Also took care of some reviewers' comments. The statistical tests are not yet fixed though.
</commit_message>
<xml_diff>
--- a/data/DesignMatrix.xlsx
+++ b/data/DesignMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F1CF4-768B-46B5-816C-D1F7E34E6699}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239C48F-1FFE-4F92-B67A-6122ABDF1E56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="245">
   <si>
     <t>Sample index</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Tissue</t>
   </si>
   <si>
-    <t>Bulk=1</t>
-  </si>
-  <si>
     <t>B cells, 3 samples from the same patient, FANTOM5</t>
   </si>
   <si>
@@ -754,6 +751,21 @@
   </si>
   <si>
     <t>Smart-Seq2</t>
+  </si>
+  <si>
+    <t>Bulk=1, Smart-Seq2 = 2</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>Lung cancer</t>
+  </si>
+  <si>
+    <t>Melanoma</t>
+  </si>
+  <si>
+    <t>No. Cells</t>
   </si>
 </sst>
 </file>
@@ -1114,14 +1126,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
   <dimension ref="B2:DC10"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="CO4" sqref="CO4"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="CV5" sqref="CV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="107" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1136,13 +1148,13 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BO2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BY2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="2:107" x14ac:dyDescent="0.25">
@@ -2060,28 +2072,28 @@
         <v>1</v>
       </c>
       <c r="CO5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CP5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CQ5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CR5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CS5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CT5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="CU5" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CV5" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CW5" s="4">
         <v>1</v>
@@ -2099,15 +2111,15 @@
         <v>1</v>
       </c>
       <c r="DB5" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="DC5" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -2427,7 +2439,7 @@
     </row>
     <row r="7" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -2587,7 +2599,7 @@
     </row>
     <row r="8" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -2907,7 +2919,7 @@
     </row>
     <row r="9" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -3227,7 +3239,7 @@
     </row>
     <row r="10" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
@@ -3371,7 +3383,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3379,7 +3391,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3389,10 +3401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,11 +3413,12 @@
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3419,13 +3432,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3438,14 +3454,15 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3458,14 +3475,15 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3478,14 +3496,15 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3498,14 +3517,15 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3518,14 +3538,15 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3538,14 +3559,15 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3558,14 +3580,15 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3578,14 +3601,15 @@
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3598,14 +3622,15 @@
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3618,14 +3643,15 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3638,14 +3664,15 @@
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3653,19 +3680,20 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3676,14 +3704,15 @@
       <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3695,11 +3724,12 @@
         <v>7</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3711,11 +3741,12 @@
         <v>7</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3726,14 +3757,15 @@
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3745,11 +3777,12 @@
         <v>7</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3761,11 +3794,12 @@
         <v>7</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3776,14 +3810,15 @@
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3795,11 +3830,12 @@
         <v>8</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3811,11 +3847,12 @@
         <v>8</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3826,14 +3863,15 @@
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3845,11 +3883,12 @@
         <v>8</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3861,11 +3900,12 @@
         <v>8</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3873,1412 +3913,1555 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G51" t="s">
         <v>125</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F51" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C62" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
+        <v>159</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
+        <v>161</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
+        <v>163</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" t="s">
         <v>168</v>
       </c>
-      <c r="C66" t="s">
-        <v>169</v>
-      </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C72" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C75" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" t="s">
         <v>200</v>
       </c>
-      <c r="C76" t="s">
-        <v>201</v>
-      </c>
       <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <v>10154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C77" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
+        <v>24384</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C78" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E78" s="1">
+        <v>30574</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C79" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E79" s="1">
+        <v>15605</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C80" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="1">
+        <v>21959</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="1">
+        <v>22371</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="1">
+        <v>24549</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="1">
+        <v>18016</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="1">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="1">
+        <v>5774</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="1">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="1">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="1">
+        <v>4764</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C89" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="1">
+        <v>4849</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C90" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="1">
+        <v>7896</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C91" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="1">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C92" t="s">
         <v>217</v>
       </c>
-      <c r="C92" t="s">
-        <v>218</v>
-      </c>
       <c r="D92" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="1">
+        <v>3600</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C93" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="1">
+        <v>8171</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C94" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="1">
+        <v>4870</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="1">
+        <v>850</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="1">
+        <v>1061</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C97" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="1">
+        <v>2145</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="1">
+        <v>4864</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="1">
+        <v>297</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C100" t="s">
         <v>228</v>
       </c>
-      <c r="C100" t="s">
-        <v>229</v>
-      </c>
       <c r="D100" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="1">
+        <v>48657</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C101" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="1">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="E102" s="1">
+        <v>10224</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="1">
+        <v>10085</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D104" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E104" s="1">
+        <v>5662</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="1">
+        <v>2040</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="1">
+        <v>512</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5289,10 +5472,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6C2E3B-6ECE-4AF1-B74E-2ADC4D0D5D0C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5302,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5310,7 +5493,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5318,7 +5501,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5326,7 +5509,31 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5339,7 +5546,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5349,7 +5556,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5357,7 +5564,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5365,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5373,7 +5580,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5381,10 +5588,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5392,7 +5599,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5400,7 +5607,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5408,7 +5615,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5416,7 +5623,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5424,7 +5631,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5437,7 +5644,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" activeCellId="1" sqref="B10 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5447,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5455,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5463,7 +5670,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5471,7 +5678,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5479,7 +5686,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5487,7 +5694,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5495,7 +5702,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5503,7 +5710,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5511,7 +5718,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5519,7 +5726,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5527,7 +5734,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5535,7 +5742,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5543,7 +5750,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>